<commit_message>
modify import button og oa-goods
</commit_message>
<xml_diff>
--- a/advanced/backend/web/template.xlsx
+++ b/advanced/backend/web/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection sqref="A1:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
show products to check
</commit_message>
<xml_diff>
--- a/advanced/backend/web/template.xlsx
+++ b/advanced/backend/web/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -786,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D80"/>
     </sheetView>
   </sheetViews>

</xml_diff>